<commit_message>
added mailer and fix excel bug
</commit_message>
<xml_diff>
--- a/summary/people counting summary.xlsx
+++ b/summary/people counting summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,21 @@
           <t>2021-11-07</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2021-11-09</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2021-11-10</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -452,6 +467,13 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -460,6 +482,13 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -468,6 +497,13 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -476,6 +512,13 @@
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -484,6 +527,13 @@
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -492,6 +542,13 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -500,6 +557,15 @@
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -508,6 +574,13 @@
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -516,6 +589,13 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -526,6 +606,13 @@
       <c r="B11" t="n">
         <v>13</v>
       </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -534,6 +621,13 @@
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -542,6 +636,11 @@
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -550,6 +649,13 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -558,6 +664,13 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -566,6 +679,13 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -574,6 +694,13 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -582,6 +709,13 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -590,6 +724,15 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>13</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -598,6 +741,13 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -606,6 +756,15 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -614,6 +773,13 @@
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -622,6 +788,13 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -630,6 +803,13 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -638,6 +818,13 @@
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>